<commit_message>
Completed all code and inserted fake data from mockroo
</commit_message>
<xml_diff>
--- a/Info340Project-XifeiWang/Milestone 01 - Database Plan/DeveloperDocument.xlsx
+++ b/Info340Project-XifeiWang/Milestone 01 - Database Plan/DeveloperDocument.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xifei/Desktop/Info340 Final/Info340Project-XifeiWang/Milestone 01 - Database Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C45EE96-E14B-454A-86E1-31703DB7FBFB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7753A319-3D5C-2349-9235-BA756D689DC5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11020" yWindow="1200" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="520" windowWidth="17180" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database Design" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="104">
   <si>
     <t>Patient Appointments Project</t>
   </si>
@@ -350,13 +350,19 @@
     <t>pDelAppointment</t>
   </si>
   <si>
-    <t>Reference from doctor table</t>
-  </si>
-  <si>
     <t>Two letter state code</t>
   </si>
   <si>
     <t>Check to be male or femle(F OR M)</t>
+  </si>
+  <si>
+    <t>Not Null,fk</t>
+  </si>
+  <si>
+    <t>Check reference from Clinic(ClinicID)</t>
+  </si>
+  <si>
+    <t>Check to match Phone pattern 206-123-1234</t>
   </si>
 </sst>
 </file>
@@ -787,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I585"/>
+  <dimension ref="A1:I589"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -931,7 +937,7 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -994,23 +1000,6 @@
       </c>
       <c r="F13" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1131,20 +1120,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>19</v>
@@ -1266,20 +1241,6 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>19</v>
@@ -1396,20 +1357,6 @@
       </c>
       <c r="D40" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1585,7 +1532,7 @@
         <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1619,7 +1566,7 @@
         <v>65</v>
       </c>
       <c r="F58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2219,7 +2166,7 @@
         <v>24</v>
       </c>
       <c r="F101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -2240,37 +2187,40 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
+      <c r="A103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" t="s">
+        <v>101</v>
+      </c>
+      <c r="F103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E103" s="3" t="s">
+      <c r="D104" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F103" s="3" t="s">
+      <c r="F104" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>7</v>
-      </c>
-      <c r="B104" t="s">
-        <v>74</v>
-      </c>
-      <c r="C104" t="s">
-        <v>8</v>
-      </c>
-      <c r="D104" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -2278,10 +2228,10 @@
         <v>7</v>
       </c>
       <c r="B105" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C105" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D105" t="s">
         <v>30</v>
@@ -2292,7 +2242,7 @@
         <v>7</v>
       </c>
       <c r="B106" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C106" t="s">
         <v>56</v>
@@ -2306,7 +2256,7 @@
         <v>7</v>
       </c>
       <c r="B107" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C107" t="s">
         <v>56</v>
@@ -2320,7 +2270,7 @@
         <v>7</v>
       </c>
       <c r="B108" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C108" t="s">
         <v>56</v>
@@ -2334,7 +2284,7 @@
         <v>7</v>
       </c>
       <c r="B109" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C109" t="s">
         <v>56</v>
@@ -2348,10 +2298,10 @@
         <v>7</v>
       </c>
       <c r="B110" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C110" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D110" t="s">
         <v>30</v>
@@ -2362,64 +2312,61 @@
         <v>7</v>
       </c>
       <c r="B111" t="s">
+        <v>85</v>
+      </c>
+      <c r="C111" t="s">
+        <v>47</v>
+      </c>
+      <c r="D111" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>7</v>
+      </c>
+      <c r="B112" t="s">
         <v>86</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>46</v>
       </c>
-      <c r="D111" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>18</v>
+      <c r="D112" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B113" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
       </c>
       <c r="D113" t="s">
-        <v>51</v>
-      </c>
-      <c r="F113" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>25</v>
-      </c>
-      <c r="B114" t="s">
-        <v>80</v>
-      </c>
-      <c r="C114" t="s">
-        <v>56</v>
-      </c>
-      <c r="D114" t="s">
-        <v>32</v>
+      <c r="A114" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -2427,13 +2374,16 @@
         <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C115" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D115" t="s">
-        <v>32</v>
+        <v>51</v>
+      </c>
+      <c r="F115" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -2441,7 +2391,7 @@
         <v>25</v>
       </c>
       <c r="B116" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C116" t="s">
         <v>56</v>
@@ -2455,7 +2405,7 @@
         <v>25</v>
       </c>
       <c r="B117" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C117" t="s">
         <v>56</v>
@@ -2469,7 +2419,7 @@
         <v>25</v>
       </c>
       <c r="B118" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C118" t="s">
         <v>56</v>
@@ -2483,10 +2433,10 @@
         <v>25</v>
       </c>
       <c r="B119" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C119" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D119" t="s">
         <v>32</v>
@@ -2497,33 +2447,27 @@
         <v>25</v>
       </c>
       <c r="B120" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C120" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D120" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>18</v>
+      <c r="A121" t="s">
+        <v>25</v>
+      </c>
+      <c r="B121" t="s">
+        <v>85</v>
+      </c>
+      <c r="C121" t="s">
+        <v>47</v>
+      </c>
+      <c r="D121" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -2531,13 +2475,13 @@
         <v>25</v>
       </c>
       <c r="B122" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C122" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D122" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -2545,27 +2489,33 @@
         <v>25</v>
       </c>
       <c r="B123" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="C123" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D123" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>25</v>
-      </c>
-      <c r="B124" t="s">
-        <v>81</v>
-      </c>
-      <c r="C124" t="s">
-        <v>56</v>
-      </c>
-      <c r="D124" t="s">
-        <v>32</v>
+      <c r="A124" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -2573,13 +2523,13 @@
         <v>25</v>
       </c>
       <c r="B125" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C125" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D125" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -2587,7 +2537,7 @@
         <v>25</v>
       </c>
       <c r="B126" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C126" t="s">
         <v>56</v>
@@ -2601,7 +2551,7 @@
         <v>25</v>
       </c>
       <c r="B127" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C127" t="s">
         <v>56</v>
@@ -2615,10 +2565,10 @@
         <v>25</v>
       </c>
       <c r="B128" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C128" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D128" t="s">
         <v>32</v>
@@ -2629,33 +2579,27 @@
         <v>25</v>
       </c>
       <c r="B129" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C129" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D129" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E130" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>18</v>
+      <c r="A130" t="s">
+        <v>25</v>
+      </c>
+      <c r="B130" t="s">
+        <v>84</v>
+      </c>
+      <c r="C130" t="s">
+        <v>56</v>
+      </c>
+      <c r="D130" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -2663,104 +2607,110 @@
         <v>25</v>
       </c>
       <c r="B131" t="s">
+        <v>85</v>
+      </c>
+      <c r="C131" t="s">
+        <v>47</v>
+      </c>
+      <c r="D131" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>25</v>
+      </c>
+      <c r="B132" t="s">
+        <v>86</v>
+      </c>
+      <c r="C132" t="s">
+        <v>46</v>
+      </c>
+      <c r="D132" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>25</v>
+      </c>
+      <c r="B133" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133" t="s">
+        <v>8</v>
+      </c>
+      <c r="D133" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>25</v>
+      </c>
+      <c r="B135" t="s">
         <v>74</v>
       </c>
-      <c r="C131" t="s">
-        <v>8</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="C135" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136" s="6" t="s">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="B140" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C140" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D136" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E136" s="6" t="s">
+      <c r="D140" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E140" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F136" s="3"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>7</v>
-      </c>
-      <c r="B137" t="s">
-        <v>49</v>
-      </c>
-      <c r="C137" t="s">
-        <v>8</v>
-      </c>
-      <c r="D137" t="s">
-        <v>22</v>
-      </c>
-      <c r="F137" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>7</v>
-      </c>
-      <c r="B138" t="s">
-        <v>89</v>
-      </c>
-      <c r="C138" t="s">
-        <v>90</v>
-      </c>
-      <c r="D138" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>7</v>
-      </c>
-      <c r="B139" t="s">
-        <v>91</v>
-      </c>
-      <c r="C139" t="s">
-        <v>56</v>
-      </c>
-      <c r="D139" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>7</v>
-      </c>
-      <c r="B140" t="s">
-        <v>92</v>
-      </c>
-      <c r="C140" t="s">
-        <v>56</v>
-      </c>
-      <c r="D140" t="s">
-        <v>24</v>
-      </c>
+      <c r="F140" s="3"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>7</v>
       </c>
       <c r="B141" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="C141" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D141" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="F141" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -2768,16 +2718,13 @@
         <v>7</v>
       </c>
       <c r="B142" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C142" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D142" t="s">
-        <v>65</v>
-      </c>
-      <c r="F142" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
@@ -2785,13 +2732,13 @@
         <v>7</v>
       </c>
       <c r="B143" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C143" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D143" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -2799,33 +2746,27 @@
         <v>7</v>
       </c>
       <c r="B144" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C144" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D144" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F145" s="3" t="s">
-        <v>18</v>
+      <c r="A145" t="s">
+        <v>7</v>
+      </c>
+      <c r="B145" t="s">
+        <v>93</v>
+      </c>
+      <c r="C145" t="s">
+        <v>47</v>
+      </c>
+      <c r="D145" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -2833,13 +2774,16 @@
         <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C146" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D146" t="s">
-        <v>30</v>
+        <v>65</v>
+      </c>
+      <c r="F146" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
@@ -2847,13 +2791,13 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C147" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D147" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
@@ -2861,27 +2805,33 @@
         <v>7</v>
       </c>
       <c r="B148" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="C148" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D148" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>7</v>
-      </c>
-      <c r="B149" t="s">
-        <v>92</v>
-      </c>
-      <c r="C149" t="s">
-        <v>56</v>
-      </c>
-      <c r="D149" t="s">
-        <v>30</v>
+      <c r="A149" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
@@ -2889,10 +2839,10 @@
         <v>7</v>
       </c>
       <c r="B150" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="C150" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D150" t="s">
         <v>30</v>
@@ -2903,10 +2853,10 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C151" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D151" t="s">
         <v>30</v>
@@ -2917,10 +2867,10 @@
         <v>7</v>
       </c>
       <c r="B152" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C152" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D152" t="s">
         <v>30</v>
@@ -2931,33 +2881,27 @@
         <v>7</v>
       </c>
       <c r="B153" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C153" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D153" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D154" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F154" s="3" t="s">
-        <v>18</v>
+      <c r="A154" t="s">
+        <v>7</v>
+      </c>
+      <c r="B154" t="s">
+        <v>93</v>
+      </c>
+      <c r="C154" t="s">
+        <v>47</v>
+      </c>
+      <c r="D154" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -2965,16 +2909,13 @@
         <v>7</v>
       </c>
       <c r="B155" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C155" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D155" t="s">
-        <v>51</v>
-      </c>
-      <c r="F155" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -2982,13 +2923,13 @@
         <v>7</v>
       </c>
       <c r="B156" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C156" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D156" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -2996,27 +2937,33 @@
         <v>7</v>
       </c>
       <c r="B157" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="C157" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D157" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>7</v>
-      </c>
-      <c r="B158" t="s">
-        <v>92</v>
-      </c>
-      <c r="C158" t="s">
-        <v>56</v>
-      </c>
-      <c r="D158" t="s">
-        <v>32</v>
+      <c r="A158" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
@@ -3024,13 +2971,16 @@
         <v>7</v>
       </c>
       <c r="B159" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="C159" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D159" t="s">
-        <v>32</v>
+        <v>51</v>
+      </c>
+      <c r="F159" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -3038,10 +2988,10 @@
         <v>7</v>
       </c>
       <c r="B160" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C160" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D160" t="s">
         <v>32</v>
@@ -3052,10 +3002,10 @@
         <v>7</v>
       </c>
       <c r="B161" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C161" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D161" t="s">
         <v>32</v>
@@ -3066,33 +3016,27 @@
         <v>7</v>
       </c>
       <c r="B162" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C162" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D162" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A163" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F163" s="3" t="s">
-        <v>18</v>
+      <c r="A163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B163" t="s">
+        <v>93</v>
+      </c>
+      <c r="C163" t="s">
+        <v>47</v>
+      </c>
+      <c r="D163" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
@@ -3100,13 +3044,13 @@
         <v>7</v>
       </c>
       <c r="B164" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C164" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D164" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
@@ -3114,10 +3058,10 @@
         <v>7</v>
       </c>
       <c r="B165" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C165" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="D165" t="s">
         <v>32</v>
@@ -3128,27 +3072,33 @@
         <v>7</v>
       </c>
       <c r="B166" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="C166" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D166" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>7</v>
-      </c>
-      <c r="B167" t="s">
-        <v>92</v>
-      </c>
-      <c r="C167" t="s">
-        <v>56</v>
-      </c>
-      <c r="D167" t="s">
-        <v>32</v>
+      <c r="A167" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
@@ -3156,13 +3106,13 @@
         <v>7</v>
       </c>
       <c r="B168" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="C168" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D168" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
@@ -3170,10 +3120,10 @@
         <v>7</v>
       </c>
       <c r="B169" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C169" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D169" t="s">
         <v>32</v>
@@ -3184,10 +3134,10 @@
         <v>7</v>
       </c>
       <c r="B170" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C170" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D170" t="s">
         <v>32</v>
@@ -3198,146 +3148,137 @@
         <v>7</v>
       </c>
       <c r="B171" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C171" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D171" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A172" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D172" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F172" s="3" t="s">
-        <v>18</v>
+      <c r="A172" t="s">
+        <v>7</v>
+      </c>
+      <c r="B172" t="s">
+        <v>93</v>
+      </c>
+      <c r="C172" t="s">
+        <v>47</v>
+      </c>
+      <c r="D172" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B173" t="s">
+        <v>94</v>
+      </c>
+      <c r="C173" t="s">
+        <v>46</v>
+      </c>
+      <c r="D173" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>7</v>
+      </c>
+      <c r="B174" t="s">
+        <v>74</v>
+      </c>
+      <c r="C174" t="s">
+        <v>8</v>
+      </c>
+      <c r="D174" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B175" t="s">
+        <v>54</v>
+      </c>
+      <c r="C175" t="s">
+        <v>8</v>
+      </c>
+      <c r="D175" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>25</v>
+      </c>
+      <c r="B177" t="s">
         <v>49</v>
       </c>
-      <c r="C173" t="s">
-        <v>8</v>
-      </c>
-      <c r="D173" t="s">
+      <c r="C177" t="s">
+        <v>8</v>
+      </c>
+      <c r="D177" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="456" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D456" t="s">
-        <v>4</v>
-      </c>
-      <c r="E456" t="s">
-        <v>21</v>
-      </c>
-      <c r="F456" t="s">
-        <v>5</v>
-      </c>
-      <c r="G456" t="s">
-        <v>30</v>
-      </c>
-      <c r="H456" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="457" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D457" t="s">
-        <v>6</v>
-      </c>
-      <c r="E457" t="s">
-        <v>35</v>
-      </c>
-      <c r="F457" t="s">
-        <v>5</v>
-      </c>
-      <c r="G457" t="s">
-        <v>30</v>
-      </c>
-      <c r="H457" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="458" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D458" t="s">
-        <v>7</v>
-      </c>
-      <c r="E458" t="s">
-        <v>9</v>
-      </c>
-      <c r="F458" t="s">
-        <v>8</v>
-      </c>
-      <c r="G458" t="s">
-        <v>22</v>
-      </c>
-      <c r="I458" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="459" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D459" t="s">
-        <v>7</v>
-      </c>
-      <c r="E459" t="s">
-        <v>10</v>
-      </c>
-      <c r="F459" t="s">
-        <v>15</v>
-      </c>
-      <c r="G459" t="s">
-        <v>45</v>
-      </c>
-      <c r="I459" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="460" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D460" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E460" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="F460" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G460" t="s">
-        <v>38</v>
-      </c>
-      <c r="I460" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="H460" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="461" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D461" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E461" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="F461" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G461" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="H461" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="462" spans="4:9" x14ac:dyDescent="0.2">
@@ -3345,13 +3286,16 @@
         <v>7</v>
       </c>
       <c r="E462" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F462" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G462" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="I462" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="463" spans="4:9" x14ac:dyDescent="0.2">
@@ -3359,16 +3303,16 @@
         <v>7</v>
       </c>
       <c r="E463" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F463" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G463" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="I463" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="464" spans="4:9" x14ac:dyDescent="0.2">
@@ -3376,16 +3320,16 @@
         <v>7</v>
       </c>
       <c r="E464" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F464" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="G464" t="s">
         <v>38</v>
       </c>
       <c r="I464" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="465" spans="4:9" x14ac:dyDescent="0.2">
@@ -3393,33 +3337,27 @@
         <v>7</v>
       </c>
       <c r="E465" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="F465" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G465" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="466" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D466" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E466" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F466" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G466" t="s">
-        <v>30</v>
-      </c>
-      <c r="H466" t="s">
-        <v>28</v>
-      </c>
-      <c r="I466" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="467" spans="4:9" x14ac:dyDescent="0.2">
@@ -3427,13 +3365,16 @@
         <v>7</v>
       </c>
       <c r="E467" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F467" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="G467" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="I467" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="468" spans="4:9" x14ac:dyDescent="0.2">
@@ -3441,13 +3382,16 @@
         <v>7</v>
       </c>
       <c r="E468" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F468" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G468" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="I468" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="469" spans="4:9" x14ac:dyDescent="0.2">
@@ -3455,27 +3399,33 @@
         <v>7</v>
       </c>
       <c r="E469" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F469" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G469" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="470" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D470" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E470" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F470" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G470" t="s">
         <v>30</v>
+      </c>
+      <c r="H470" t="s">
+        <v>28</v>
+      </c>
+      <c r="I470" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="471" spans="4:9" x14ac:dyDescent="0.2">
@@ -3483,10 +3433,10 @@
         <v>7</v>
       </c>
       <c r="E471" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F471" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G471" t="s">
         <v>30</v>
@@ -3497,10 +3447,10 @@
         <v>7</v>
       </c>
       <c r="E472" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F472" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G472" t="s">
         <v>30</v>
@@ -3511,10 +3461,10 @@
         <v>7</v>
       </c>
       <c r="E473" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F473" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="G473" t="s">
         <v>30</v>
@@ -3525,10 +3475,10 @@
         <v>7</v>
       </c>
       <c r="E474" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="F474" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G474" t="s">
         <v>30</v>
@@ -3536,81 +3486,78 @@
     </row>
     <row r="475" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D475" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E475" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F475" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G475" t="s">
         <v>30</v>
-      </c>
-      <c r="H475" t="s">
-        <v>29</v>
-      </c>
-      <c r="I475" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="476" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D476" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E476" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F476" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="G476" t="s">
-        <v>51</v>
-      </c>
-      <c r="I476" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="477" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D477" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E477" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F477" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G477" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="478" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D478" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E478" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F478" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G478" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="479" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D479" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E479" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F479" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G479" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="H479" t="s">
+        <v>29</v>
+      </c>
+      <c r="I479" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="480" spans="4:9" x14ac:dyDescent="0.2">
@@ -3618,13 +3565,16 @@
         <v>25</v>
       </c>
       <c r="E480" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F480" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G480" t="s">
-        <v>32</v>
+        <v>51</v>
+      </c>
+      <c r="I480" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="481" spans="4:9" x14ac:dyDescent="0.2">
@@ -3632,10 +3582,10 @@
         <v>25</v>
       </c>
       <c r="E481" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F481" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G481" t="s">
         <v>32</v>
@@ -3646,10 +3596,10 @@
         <v>25</v>
       </c>
       <c r="E482" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F482" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="G482" t="s">
         <v>32</v>
@@ -3660,33 +3610,27 @@
         <v>25</v>
       </c>
       <c r="E483" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="F483" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G483" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="484" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D484" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E484" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F484" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G484" t="s">
-        <v>30</v>
-      </c>
-      <c r="H484" t="s">
-        <v>29</v>
-      </c>
-      <c r="I484" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="485" spans="4:9" x14ac:dyDescent="0.2">
@@ -3694,10 +3638,10 @@
         <v>25</v>
       </c>
       <c r="E485" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F485" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="G485" t="s">
         <v>32</v>
@@ -3708,10 +3652,10 @@
         <v>25</v>
       </c>
       <c r="E486" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F486" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G486" t="s">
         <v>32</v>
@@ -3722,27 +3666,33 @@
         <v>25</v>
       </c>
       <c r="E487" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F487" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G487" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="488" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D488" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E488" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F488" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G488" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="H488" t="s">
+        <v>29</v>
+      </c>
+      <c r="I488" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="489" spans="4:9" x14ac:dyDescent="0.2">
@@ -3750,10 +3700,10 @@
         <v>25</v>
       </c>
       <c r="E489" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F489" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G489" t="s">
         <v>32</v>
@@ -3764,10 +3714,10 @@
         <v>25</v>
       </c>
       <c r="E490" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F490" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G490" t="s">
         <v>32</v>
@@ -3778,10 +3728,10 @@
         <v>25</v>
       </c>
       <c r="E491" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F491" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="G491" t="s">
         <v>32</v>
@@ -3792,33 +3742,27 @@
         <v>25</v>
       </c>
       <c r="E492" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="F492" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G492" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="493" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D493" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E493" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="F493" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G493" t="s">
-        <v>30</v>
-      </c>
-      <c r="H493" t="s">
-        <v>29</v>
-      </c>
-      <c r="I493" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="494" spans="4:9" x14ac:dyDescent="0.2">
@@ -3826,92 +3770,92 @@
         <v>25</v>
       </c>
       <c r="E494" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F494" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="G494" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="495" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D495" t="s">
+        <v>25</v>
+      </c>
+      <c r="E495" t="s">
+        <v>14</v>
+      </c>
+      <c r="F495" t="s">
+        <v>46</v>
+      </c>
+      <c r="G495" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="496" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D496" t="s">
+        <v>25</v>
+      </c>
+      <c r="E496" t="s">
+        <v>49</v>
+      </c>
+      <c r="F496" t="s">
+        <v>8</v>
+      </c>
+      <c r="G496" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="497" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D497" t="s">
+        <v>19</v>
+      </c>
+      <c r="E497" t="s">
+        <v>43</v>
+      </c>
+      <c r="F497" t="s">
+        <v>5</v>
+      </c>
+      <c r="G497" t="s">
+        <v>30</v>
+      </c>
+      <c r="H497" t="s">
+        <v>29</v>
+      </c>
+      <c r="I497" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="498" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D498" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E498" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="F498" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G498" t="s">
-        <v>30</v>
-      </c>
-      <c r="H498" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="499" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D499" t="s">
-        <v>7</v>
-      </c>
-      <c r="E499" t="s">
-        <v>54</v>
-      </c>
-      <c r="F499" t="s">
-        <v>8</v>
-      </c>
-      <c r="G499" t="s">
-        <v>22</v>
-      </c>
-      <c r="I499" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="500" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D500" t="s">
-        <v>7</v>
-      </c>
-      <c r="E500" t="s">
-        <v>55</v>
-      </c>
-      <c r="F500" t="s">
-        <v>56</v>
-      </c>
-      <c r="G500" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="501" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D501" t="s">
-        <v>7</v>
-      </c>
-      <c r="E501" t="s">
-        <v>57</v>
-      </c>
-      <c r="F501" t="s">
-        <v>56</v>
-      </c>
-      <c r="G501" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="502" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D502" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E502" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F502" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G502" t="s">
-        <v>59</v>
-      </c>
-      <c r="I502" t="s">
-        <v>60</v>
+        <v>30</v>
+      </c>
+      <c r="H502" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="503" spans="4:9" x14ac:dyDescent="0.2">
@@ -3919,13 +3863,16 @@
         <v>7</v>
       </c>
       <c r="E503" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F503" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G503" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="I503" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="504" spans="4:9" x14ac:dyDescent="0.2">
@@ -3933,7 +3880,7 @@
         <v>7</v>
       </c>
       <c r="E504" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F504" t="s">
         <v>56</v>
@@ -3947,10 +3894,10 @@
         <v>7</v>
       </c>
       <c r="E505" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F505" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G505" t="s">
         <v>24</v>
@@ -3961,36 +3908,30 @@
         <v>7</v>
       </c>
       <c r="E506" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F506" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G506" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I506" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="507" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D507" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E507" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F507" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G507" t="s">
-        <v>30</v>
-      </c>
-      <c r="H507" t="s">
-        <v>28</v>
-      </c>
-      <c r="I507" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="508" spans="4:9" x14ac:dyDescent="0.2">
@@ -3998,13 +3939,13 @@
         <v>7</v>
       </c>
       <c r="E508" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F508" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="G508" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="509" spans="4:9" x14ac:dyDescent="0.2">
@@ -4012,13 +3953,13 @@
         <v>7</v>
       </c>
       <c r="E509" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F509" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G509" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="510" spans="4:9" x14ac:dyDescent="0.2">
@@ -4026,27 +3967,36 @@
         <v>7</v>
       </c>
       <c r="E510" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F510" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G510" t="s">
-        <v>30</v>
+        <v>65</v>
+      </c>
+      <c r="I510" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="511" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D511" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E511" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F511" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G511" t="s">
         <v>30</v>
+      </c>
+      <c r="H511" t="s">
+        <v>28</v>
+      </c>
+      <c r="I511" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="512" spans="4:9" x14ac:dyDescent="0.2">
@@ -4054,10 +4004,10 @@
         <v>7</v>
       </c>
       <c r="E512" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F512" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G512" t="s">
         <v>30</v>
@@ -4068,7 +4018,7 @@
         <v>7</v>
       </c>
       <c r="E513" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F513" t="s">
         <v>56</v>
@@ -4082,10 +4032,10 @@
         <v>7</v>
       </c>
       <c r="E514" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F514" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G514" t="s">
         <v>30</v>
@@ -4096,10 +4046,10 @@
         <v>7</v>
       </c>
       <c r="E515" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F515" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G515" t="s">
         <v>30</v>
@@ -4107,81 +4057,78 @@
     </row>
     <row r="516" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D516" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E516" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F516" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G516" t="s">
         <v>30</v>
-      </c>
-      <c r="H516" t="s">
-        <v>29</v>
-      </c>
-      <c r="I516" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="517" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D517" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E517" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F517" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="G517" t="s">
-        <v>51</v>
-      </c>
-      <c r="I517" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="518" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D518" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E518" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F518" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G518" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="519" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D519" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E519" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F519" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G519" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="520" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D520" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E520" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="F520" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G520" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="H520" t="s">
+        <v>29</v>
+      </c>
+      <c r="I520" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="521" spans="4:9" x14ac:dyDescent="0.2">
@@ -4189,13 +4136,16 @@
         <v>25</v>
       </c>
       <c r="E521" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F521" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G521" t="s">
-        <v>32</v>
+        <v>51</v>
+      </c>
+      <c r="I521" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="522" spans="4:9" x14ac:dyDescent="0.2">
@@ -4203,7 +4153,7 @@
         <v>25</v>
       </c>
       <c r="E522" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F522" t="s">
         <v>56</v>
@@ -4217,10 +4167,10 @@
         <v>25</v>
       </c>
       <c r="E523" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F523" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G523" t="s">
         <v>32</v>
@@ -4231,10 +4181,10 @@
         <v>25</v>
       </c>
       <c r="E524" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F524" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G524" t="s">
         <v>32</v>
@@ -4242,22 +4192,16 @@
     </row>
     <row r="525" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D525" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E525" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F525" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G525" t="s">
-        <v>30</v>
-      </c>
-      <c r="H525" t="s">
-        <v>29</v>
-      </c>
-      <c r="I525" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="526" spans="4:9" x14ac:dyDescent="0.2">
@@ -4265,13 +4209,13 @@
         <v>25</v>
       </c>
       <c r="E526" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F526" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="G526" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
     </row>
     <row r="527" spans="4:9" x14ac:dyDescent="0.2">
@@ -4279,10 +4223,10 @@
         <v>25</v>
       </c>
       <c r="E527" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F527" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G527" t="s">
         <v>32</v>
@@ -4293,10 +4237,10 @@
         <v>25</v>
       </c>
       <c r="E528" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F528" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G528" t="s">
         <v>32</v>
@@ -4304,16 +4248,22 @@
     </row>
     <row r="529" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D529" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E529" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="F529" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G529" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="H529" t="s">
+        <v>29</v>
+      </c>
+      <c r="I529" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="530" spans="4:9" x14ac:dyDescent="0.2">
@@ -4321,13 +4271,13 @@
         <v>25</v>
       </c>
       <c r="E530" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F530" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G530" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="531" spans="4:9" x14ac:dyDescent="0.2">
@@ -4335,7 +4285,7 @@
         <v>25</v>
       </c>
       <c r="E531" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F531" t="s">
         <v>56</v>
@@ -4349,10 +4299,10 @@
         <v>25</v>
       </c>
       <c r="E532" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F532" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G532" t="s">
         <v>32</v>
@@ -4363,10 +4313,10 @@
         <v>25</v>
       </c>
       <c r="E533" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F533" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G533" t="s">
         <v>32</v>
@@ -4374,22 +4324,16 @@
     </row>
     <row r="534" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D534" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E534" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F534" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G534" t="s">
-        <v>30</v>
-      </c>
-      <c r="H534" t="s">
-        <v>29</v>
-      </c>
-      <c r="I534" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="535" spans="4:9" x14ac:dyDescent="0.2">
@@ -4397,92 +4341,92 @@
         <v>25</v>
       </c>
       <c r="E535" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F535" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="G535" t="s">
-        <v>72</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="536" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D536" t="s">
+        <v>25</v>
+      </c>
+      <c r="E536" t="s">
+        <v>63</v>
+      </c>
+      <c r="F536" t="s">
+        <v>47</v>
+      </c>
+      <c r="G536" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="537" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D537" t="s">
+        <v>25</v>
+      </c>
+      <c r="E537" t="s">
+        <v>64</v>
+      </c>
+      <c r="F537" t="s">
+        <v>46</v>
+      </c>
+      <c r="G537" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="538" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D538" t="s">
+        <v>19</v>
+      </c>
+      <c r="E538" t="s">
+        <v>71</v>
+      </c>
+      <c r="F538" t="s">
+        <v>5</v>
+      </c>
+      <c r="G538" t="s">
+        <v>30</v>
+      </c>
+      <c r="H538" t="s">
+        <v>29</v>
+      </c>
+      <c r="I538" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="539" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D539" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E539" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="F539" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G539" t="s">
-        <v>30</v>
-      </c>
-      <c r="H539" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="540" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D540" t="s">
-        <v>7</v>
-      </c>
-      <c r="E540" t="s">
-        <v>54</v>
-      </c>
-      <c r="F540" t="s">
-        <v>8</v>
-      </c>
-      <c r="G540" t="s">
-        <v>22</v>
-      </c>
-      <c r="I540" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="541" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D541" t="s">
-        <v>7</v>
-      </c>
-      <c r="E541" t="s">
-        <v>55</v>
-      </c>
-      <c r="F541" t="s">
-        <v>56</v>
-      </c>
-      <c r="G541" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="542" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D542" t="s">
-        <v>7</v>
-      </c>
-      <c r="E542" t="s">
-        <v>57</v>
-      </c>
-      <c r="F542" t="s">
-        <v>56</v>
-      </c>
-      <c r="G542" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="543" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D543" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E543" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F543" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G543" t="s">
-        <v>59</v>
-      </c>
-      <c r="I543" t="s">
-        <v>60</v>
+        <v>30</v>
+      </c>
+      <c r="H543" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="544" spans="4:9" x14ac:dyDescent="0.2">
@@ -4490,13 +4434,16 @@
         <v>7</v>
       </c>
       <c r="E544" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F544" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G544" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="I544" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="545" spans="4:9" x14ac:dyDescent="0.2">
@@ -4504,7 +4451,7 @@
         <v>7</v>
       </c>
       <c r="E545" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F545" t="s">
         <v>56</v>
@@ -4518,10 +4465,10 @@
         <v>7</v>
       </c>
       <c r="E546" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F546" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G546" t="s">
         <v>24</v>
@@ -4532,36 +4479,44 @@
         <v>7</v>
       </c>
       <c r="E547" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F547" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G547" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I547" t="s">
-        <v>66</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="548" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D548" t="s">
+        <v>7</v>
+      </c>
+      <c r="E548" t="s">
+        <v>61</v>
+      </c>
+      <c r="F548" t="s">
+        <v>56</v>
+      </c>
+      <c r="G548" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="549" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D549" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E549" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F549" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G549" t="s">
-        <v>30</v>
-      </c>
-      <c r="H549" t="s">
-        <v>28</v>
-      </c>
-      <c r="I549" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="550" spans="4:9" x14ac:dyDescent="0.2">
@@ -4569,13 +4524,13 @@
         <v>7</v>
       </c>
       <c r="E550" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F550" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="G550" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="551" spans="4:9" x14ac:dyDescent="0.2">
@@ -4583,41 +4538,36 @@
         <v>7</v>
       </c>
       <c r="E551" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F551" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G551" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="552" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D552" t="s">
-        <v>7</v>
-      </c>
-      <c r="E552" t="s">
-        <v>57</v>
-      </c>
-      <c r="F552" t="s">
-        <v>56</v>
-      </c>
-      <c r="G552" t="s">
-        <v>30</v>
+        <v>65</v>
+      </c>
+      <c r="I551" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="553" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D553" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E553" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F553" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G553" t="s">
         <v>30</v>
+      </c>
+      <c r="H553" t="s">
+        <v>28</v>
+      </c>
+      <c r="I553" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="554" spans="4:9" x14ac:dyDescent="0.2">
@@ -4625,10 +4575,10 @@
         <v>7</v>
       </c>
       <c r="E554" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F554" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G554" t="s">
         <v>30</v>
@@ -4639,7 +4589,7 @@
         <v>7</v>
       </c>
       <c r="E555" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F555" t="s">
         <v>56</v>
@@ -4653,10 +4603,10 @@
         <v>7</v>
       </c>
       <c r="E556" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F556" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G556" t="s">
         <v>30</v>
@@ -4667,92 +4617,89 @@
         <v>7</v>
       </c>
       <c r="E557" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F557" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G557" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="558" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D558" t="s">
+        <v>7</v>
+      </c>
+      <c r="E558" t="s">
+        <v>61</v>
+      </c>
+      <c r="F558" t="s">
+        <v>56</v>
+      </c>
+      <c r="G558" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="559" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D559" t="s">
+        <v>7</v>
+      </c>
+      <c r="E559" t="s">
+        <v>62</v>
+      </c>
+      <c r="F559" t="s">
+        <v>56</v>
+      </c>
+      <c r="G559" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="560" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D560" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E560" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F560" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="G560" t="s">
         <v>30</v>
-      </c>
-      <c r="H560" t="s">
-        <v>29</v>
-      </c>
-      <c r="I560" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="561" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D561" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E561" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F561" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="G561" t="s">
-        <v>51</v>
-      </c>
-      <c r="I561" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="562" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D562" t="s">
-        <v>25</v>
-      </c>
-      <c r="E562" t="s">
-        <v>55</v>
-      </c>
-      <c r="F562" t="s">
-        <v>56</v>
-      </c>
-      <c r="G562" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="563" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D563" t="s">
-        <v>25</v>
-      </c>
-      <c r="E563" t="s">
-        <v>57</v>
-      </c>
-      <c r="F563" t="s">
-        <v>56</v>
-      </c>
-      <c r="G563" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="564" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D564" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E564" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="F564" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G564" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="H564" t="s">
+        <v>29</v>
+      </c>
+      <c r="I564" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="565" spans="4:9" x14ac:dyDescent="0.2">
@@ -4760,13 +4707,16 @@
         <v>25</v>
       </c>
       <c r="E565" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F565" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G565" t="s">
-        <v>32</v>
+        <v>51</v>
+      </c>
+      <c r="I565" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="566" spans="4:9" x14ac:dyDescent="0.2">
@@ -4774,7 +4724,7 @@
         <v>25</v>
       </c>
       <c r="E566" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F566" t="s">
         <v>56</v>
@@ -4788,10 +4738,10 @@
         <v>25</v>
       </c>
       <c r="E567" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F567" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G567" t="s">
         <v>32</v>
@@ -4802,89 +4752,89 @@
         <v>25</v>
       </c>
       <c r="E568" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F568" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G568" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="569" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D569" t="s">
+        <v>25</v>
+      </c>
+      <c r="E569" t="s">
+        <v>61</v>
+      </c>
+      <c r="F569" t="s">
+        <v>56</v>
+      </c>
+      <c r="G569" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="570" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D570" t="s">
+        <v>25</v>
+      </c>
+      <c r="E570" t="s">
+        <v>62</v>
+      </c>
+      <c r="F570" t="s">
+        <v>56</v>
+      </c>
+      <c r="G570" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="571" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D571" t="s">
+        <v>25</v>
+      </c>
+      <c r="E571" t="s">
+        <v>63</v>
+      </c>
+      <c r="F571" t="s">
+        <v>47</v>
+      </c>
+      <c r="G571" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="572" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D572" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E572" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F572" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G572" t="s">
-        <v>30</v>
-      </c>
-      <c r="H572" t="s">
-        <v>29</v>
-      </c>
-      <c r="I572" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="573" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D573" t="s">
-        <v>25</v>
-      </c>
-      <c r="E573" t="s">
-        <v>54</v>
-      </c>
-      <c r="F573" t="s">
-        <v>8</v>
-      </c>
-      <c r="G573" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="574" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D574" t="s">
-        <v>25</v>
-      </c>
-      <c r="E574" t="s">
-        <v>55</v>
-      </c>
-      <c r="F574" t="s">
-        <v>56</v>
-      </c>
-      <c r="G574" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="575" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D575" t="s">
-        <v>25</v>
-      </c>
-      <c r="E575" t="s">
-        <v>57</v>
-      </c>
-      <c r="F575" t="s">
-        <v>56</v>
-      </c>
-      <c r="G575" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="576" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D576" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E576" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="F576" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G576" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="H576" t="s">
+        <v>29</v>
+      </c>
+      <c r="I576" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="577" spans="4:9" x14ac:dyDescent="0.2">
@@ -4892,13 +4842,13 @@
         <v>25</v>
       </c>
       <c r="E577" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F577" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G577" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="578" spans="4:9" x14ac:dyDescent="0.2">
@@ -4906,7 +4856,7 @@
         <v>25</v>
       </c>
       <c r="E578" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F578" t="s">
         <v>56</v>
@@ -4920,10 +4870,10 @@
         <v>25</v>
       </c>
       <c r="E579" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F579" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G579" t="s">
         <v>32</v>
@@ -4934,46 +4884,102 @@
         <v>25</v>
       </c>
       <c r="E580" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F580" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G580" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="581" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D581" t="s">
+        <v>25</v>
+      </c>
+      <c r="E581" t="s">
+        <v>61</v>
+      </c>
+      <c r="F581" t="s">
+        <v>56</v>
+      </c>
+      <c r="G581" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="582" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D582" t="s">
+        <v>25</v>
+      </c>
+      <c r="E582" t="s">
+        <v>62</v>
+      </c>
+      <c r="F582" t="s">
+        <v>56</v>
+      </c>
+      <c r="G582" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="583" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D583" t="s">
+        <v>25</v>
+      </c>
+      <c r="E583" t="s">
+        <v>63</v>
+      </c>
+      <c r="F583" t="s">
+        <v>47</v>
+      </c>
+      <c r="G583" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="584" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D584" t="s">
+        <v>25</v>
+      </c>
+      <c r="E584" t="s">
+        <v>64</v>
+      </c>
+      <c r="F584" t="s">
+        <v>46</v>
+      </c>
+      <c r="G584" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="588" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D588" t="s">
         <v>19</v>
       </c>
-      <c r="E584" t="s">
+      <c r="E588" t="s">
         <v>71</v>
       </c>
-      <c r="F584" t="s">
+      <c r="F588" t="s">
         <v>5</v>
       </c>
-      <c r="G584" t="s">
-        <v>30</v>
-      </c>
-      <c r="H584" t="s">
+      <c r="G588" t="s">
+        <v>30</v>
+      </c>
+      <c r="H588" t="s">
         <v>29</v>
       </c>
-      <c r="I584" t="s">
+      <c r="I588" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="585" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D585" t="s">
-        <v>25</v>
-      </c>
-      <c r="E585" t="s">
+    <row r="589" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D589" t="s">
+        <v>25</v>
+      </c>
+      <c r="E589" t="s">
         <v>54</v>
       </c>
-      <c r="F585" t="s">
-        <v>8</v>
-      </c>
-      <c r="G585" t="s">
+      <c r="F589" t="s">
+        <v>8</v>
+      </c>
+      <c r="G589" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>